<commit_message>
Added Constructors to Class Ingredient plus more Storedprocedures
</commit_message>
<xml_diff>
--- a/SchemesDiagramsEtc/CRUD Diagram.xlsx
+++ b/SchemesDiagramsEtc/CRUD Diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Tutorials\Curso Programador\Course Project\SchemesDiagramsEtc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243B31B2-F89F-4E5E-BEA4-72AB3E5322A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F132745-80B1-4ECD-8B74-5E42A9604FBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98649944-44C6-450D-AC39-6FA1031C4605}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
   <si>
     <t>User</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>CRUD</t>
+  </si>
+  <si>
+    <t>Update Comment Recipe</t>
+  </si>
+  <si>
+    <t>Delete Comment Recipe</t>
   </si>
 </sst>
 </file>
@@ -493,12 +499,13 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="18" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.25">
@@ -662,7 +669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -694,7 +701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -750,7 +757,7 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -779,12 +786,21 @@
       <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -798,12 +814,21 @@
       <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>

</xml_diff>

<commit_message>
Added WinForms and Classes to manage MeasurementUnits DishTypes and CuisineTypes plus more StoredProcedures
</commit_message>
<xml_diff>
--- a/SchemesDiagramsEtc/CRUD Diagram.xlsx
+++ b/SchemesDiagramsEtc/CRUD Diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Tutorials\Curso Programador\Course Project\SchemesDiagramsEtc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\danie\Documents\Tutorials\C# Curso Programador 2019\Course Project\RecipesProject\SchemesDiagramsEtc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F132745-80B1-4ECD-8B74-5E42A9604FBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8618381A-F917-49F3-82DA-67EF3E9B1EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98649944-44C6-450D-AC39-6FA1031C4605}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98649944-44C6-450D-AC39-6FA1031C4605}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>User</t>
   </si>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>Delete Comment Recipe</t>
+  </si>
+  <si>
+    <t>Insert Dish Category</t>
+  </si>
+  <si>
+    <t>Update Dish Category</t>
+  </si>
+  <si>
+    <t>Delete Dish Category</t>
+  </si>
+  <si>
+    <t>Insert Cuisine Type</t>
+  </si>
+  <si>
+    <t>Update Cuisine Type</t>
+  </si>
+  <si>
+    <t>Delete Cuisine Type</t>
   </si>
 </sst>
 </file>
@@ -496,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5AFFB4-910A-4801-B7BF-45F128A16FE0}">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,6 +860,9 @@
       <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -855,12 +876,17 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -874,12 +900,17 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="O11" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -893,12 +924,17 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="O12" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -911,13 +947,18 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="N13" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -930,12 +971,22 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="N14" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
     </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added management of duration ranges for recipes
</commit_message>
<xml_diff>
--- a/SchemesDiagramsEtc/CRUD Diagram.xlsx
+++ b/SchemesDiagramsEtc/CRUD Diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\danie\Documents\Tutorials\C# Curso Programador 2019\Course Project\RecipesProject\SchemesDiagramsEtc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Tutorials\Curso Programador\Course Project\SchemesDiagramsEtc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8618381A-F917-49F3-82DA-67EF3E9B1EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607B5345-76BA-490A-8EB6-06BE101E154B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98649944-44C6-450D-AC39-6FA1031C4605}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98649944-44C6-450D-AC39-6FA1031C4605}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
   <si>
     <t>User</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>Delete Cuisine Type</t>
+  </si>
+  <si>
+    <t>Insert TimeRange</t>
+  </si>
+  <si>
+    <t>Update TimeRange</t>
+  </si>
+  <si>
+    <t>Delete TimeRange</t>
+  </si>
+  <si>
+    <t>Insert Ingredient</t>
+  </si>
+  <si>
+    <t>Update Ingredient</t>
+  </si>
+  <si>
+    <t>Delete Ingredient</t>
   </si>
 </sst>
 </file>
@@ -514,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5AFFB4-910A-4801-B7BF-45F128A16FE0}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="K19" sqref="K19:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,6 +1005,54 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>